<commit_message>
Add new screens + fix bugs
</commit_message>
<xml_diff>
--- a/MilkTea.xlsx
+++ b/MilkTea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MilkTea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E65EFE8-C665-46E5-96A0-28AD67EC5508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911F4F70-9F91-4648-89C2-FF48896C4B94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{B37F149E-6956-44B3-A4D9-19C02EF6CB64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B37F149E-6956-44B3-A4D9-19C02EF6CB64}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,119 @@
     <t>FAILURE</t>
   </si>
   <si>
-    <t>{
+    <t>Thêm mới sản phẩm</t>
+  </si>
+  <si>
+    <t>/items</t>
+  </si>
+  <si>
+    <t>{
+    name: String,
+    price: Number,
+    category: String,
+    image: Image
+}</t>
+  </si>
+  <si>
+    <t>Lấy danh sách sản phẩm</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin sản phẩm</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Xóa sản phẩm</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/items/:id</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>{
+    name: String,
+    price: Number,
+    category: String,
+}</t>
+  </si>
+  <si>
+    <t>Thêm mới loại sản phẩm</t>
+  </si>
+  <si>
+    <t>/categories</t>
+  </si>
+  <si>
+    <t>{
+    name: String
+}</t>
+  </si>
+  <si>
+    <t>Lấy danh sách loại sản phẩm</t>
+  </si>
+  <si>
+    <t>Đổi tên loại sản phẩm</t>
+  </si>
+  <si>
+    <t>/categories/:id</t>
+  </si>
+  <si>
+    <t>Tạo mới đơn hàng</t>
+  </si>
+  <si>
+    <t>/orders</t>
+  </si>
+  <si>
+    <t>Lấy danh sách đơn hàng dựa trên tình trạng</t>
+  </si>
+  <si>
+    <t>{
+    status: String
+}</t>
+  </si>
+  <si>
+    <t>Lấy thông tin chi tiết đơn hàng</t>
+  </si>
+  <si>
+    <t>/orders/:id</t>
+  </si>
+  <si>
+    <t>{
+    userId: String, (optional)
+    status: String
+}</t>
+  </si>
+  <si>
+    <t>Cập nhật tình trạng đơn hàng</t>
+  </si>
+  <si>
+    <t>/admins</t>
+  </si>
+  <si>
+    <t>Tạo tài khoản quản trị viên</t>
+  </si>
+  <si>
+    <t>/admins/:id</t>
+  </si>
+  <si>
+    <t>{
+    password: String
+}</t>
+  </si>
+  <si>
+    <t>Xóa tài khoản</t>
+  </si>
+  <si>
+    <t>Đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
     message: "Đăng ký tài khoản thành công",
     data: {
         _id: String,
@@ -119,11 +231,7 @@
   </si>
   <si>
     <t>{
-    message: "Tài khoản này đã tồn tại"
-}</t>
-  </si>
-  <si>
-    <t>{
+    error: false,
     message: "Đăng nhập thành công",
     data: {
         _id: String,
@@ -138,19 +246,7 @@
   </si>
   <si>
     <t>{
-    message: "Tài khoản này không tồn tại"
-}
-{
-    message: "Mật khẩu không chính xác"
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Tài khoản này không tồn tại"
-}</t>
-  </si>
-  <si>
-    <t>{
+    error: false,
     message: "Cập nhật thông tin thành công",
     data: {
         _id: String,
@@ -164,65 +260,67 @@
 }</t>
   </si>
   <si>
-    <t>Thêm mới sản phẩm</t>
-  </si>
-  <si>
-    <t>/items</t>
-  </si>
-  <si>
-    <t>{
-    name: String,
-    price: Number,
-    category: String,
-    image: Image
-}</t>
-  </si>
-  <si>
-    <t>Lấy danh sách sản phẩm</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa thông tin sản phẩm</t>
-  </si>
-  <si>
-    <t>Chỉnh sửa thông tin cá nhân</t>
-  </si>
-  <si>
-    <t>Xóa sản phẩm</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>/items/:id</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>{
-    name: String,
-    price: Number,
-    category: String,
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Sản phẩm không tồn tại"
-}</t>
-  </si>
-  <si>
-    <t>Thêm mới loại sản phẩm</t>
-  </si>
-  <si>
-    <t>/categories</t>
-  </si>
-  <si>
-    <t>{
-    name: String
-}</t>
-  </si>
-  <si>
-    <t>{
+    <t>{
+    error: false,
+    message: "Thêm sản phẩm mới thành công",
+    data: {
+        _id: String,
+        name: String,
+        price: Number,
+        category: String,
+        description: String,
+        image: String
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
+    message: "Truy xuất danh sách sản phẩm thành công",
+    data: [
+        {
+            _id: String,
+            name: String,
+            price: Number,
+            category: String,
+            description: String
+            image: String
+        },
+        ...
+    ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
+    message: "Cập nhật sản phẩm thành công",
+    data: {
+        _id: String,
+        name: String,
+        price: Number,
+        category: String,
+        description: String,
+        image: String
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
+    message: "Xóa sản phẩm thành công",
+    data: {
+        _id: String,
+        name: String,
+        price: Number,
+        category: String,
+        description: String
+        image: String
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
     message: "Tạo mới loại sản phẩm thành công",
     data: {
         _id: String,
@@ -231,10 +329,8 @@
 }</t>
   </si>
   <si>
-    <t>Lấy danh sách loại sản phẩm</t>
-  </si>
-  <si>
-    <t>{
+    <t>{
+    error: false,
     message: "Truy xuất danh sách loại sản phẩm thành công",
     data: [
         {
@@ -245,13 +341,8 @@
 }</t>
   </si>
   <si>
-    <t>Đổi tên loại sản phẩm</t>
-  </si>
-  <si>
-    <t>/categories/:id</t>
-  </si>
-  <si>
-    <t>{
+    <t>{
+    error: false,
     message: "Đổi tên loại sản phẩm thành công",
     data: {
         _id: String,
@@ -261,83 +352,7 @@
   </si>
   <si>
     <t>{
-    message: "Loại sản phẩm không tồn tại"
-}</t>
-  </si>
-  <si>
-    <t>Tạo mới đơn hàng</t>
-  </si>
-  <si>
-    <t>/orders</t>
-  </si>
-  <si>
-    <t>Lấy danh sách đơn hàng dựa trên tình trạng</t>
-  </si>
-  <si>
-    <t>{
-    status: String
-}</t>
-  </si>
-  <si>
-    <t>{
-    user: String,
-    phone: String,
-    address: String,
-    details: [
-        {
-            name: String,
-            unitPrice: Number,
-            quantity: Number
-        },
-        ...
-    ]        
-}</t>
-  </si>
-  <si>
-    <t>Lấy thông tin chi tiết đơn hàng</t>
-  </si>
-  <si>
-    <t>/orders/:id</t>
-  </si>
-  <si>
-    <t>{
-    userId: String, (optional)
-    status: String
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Đơn hàng không tồn tại"
-}</t>
-  </si>
-  <si>
-    <t>Cập nhật tình trạng đơn hàng</t>
-  </si>
-  <si>
-    <t>{
-    message: "Tạo mới đơn hàng thành công",
-    data: {
-        _id: String,
-        user: String,
-        phone: String,
-        address: String,
-        totalPrice: Number,
-        status: "waiting",
-        details: [
-            {
-                name: String,
-                unitPrice: Number,
-                quantity: Number,
-                totalPrice: Number
-            },
-            ...
-        ],
-        createdAt: Date
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
+    error: false,
     message: "Truy xuất danh sách đơn hàng thành công",
     data: [
         {
@@ -355,6 +370,7 @@
   </si>
   <si>
     <t>{
+    error: false,
     message: "Truy xuất thông tin chi tiết đơn hàng thành công",
     data: {
         _id: String,
@@ -378,13 +394,8 @@
 }</t>
   </si>
   <si>
-    <t>/admins</t>
-  </si>
-  <si>
-    <t>Tạo tài khoản quản trị viên</t>
-  </si>
-  <si>
-    <t>{
+    <t>{
+    error: false,
     message: "Tạo tài khoản mới thành công",
     data: {
         _id: String,
@@ -395,6 +406,7 @@
   </si>
   <si>
     <t>{
+    error: false,
     message: "Truy xuất danh sách quản trị viên thành công",
     data: [
         {
@@ -406,23 +418,19 @@
 }</t>
   </si>
   <si>
-    <t>/admins/:id</t>
-  </si>
-  <si>
-    <t>{
-    password: String
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Tài khoản không tồn tại"
-}</t>
-  </si>
-  <si>
-    <t>Xóa tài khoản</t>
-  </si>
-  <si>
-    <t>{
+    <t>{
+    error: false,
+    message: "Đổi mật khẩu thành công",
+    data: {
+        _id: String,
+        username: String,
+        password: String
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
     message: "Xóa tài khoản thành công",
     data: {
         _id: String,
@@ -433,69 +441,87 @@
   </si>
   <si>
     <t>{
-    message: "Thêm sản phẩm mới thành công",
+    error: true,
+    message: "Tài khoản này đã tồn tại"
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: true,
+    message: "Tài khoản này không tồn tại"
+}
+hoặc
+{
+    error: true,
+    message: "Mật khẩu không chính xác"
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: true,
+    message: "Tài khoản này không tồn tại"
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: true,
+    message: "Sản phẩm không tồn tại"
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: true,
+    message: "Loại sản phẩm không tồn tại"
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: true,
+    message: "Đơn hàng không tồn tại"
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: true,
+    message: "Tài khoản không tồn tại"
+}</t>
+  </si>
+  <si>
+    <t>{
+    name: String,
+    phone: String,
+    address: String,
+    details: [
+        {
+            name: String,
+            unitPrice: Number,
+            quantity: Number
+        },
+        ...
+    ]        
+}</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
+    message: "Tạo mới đơn hàng thành công",
     data: {
         _id: String,
         name: String,
-        price: Number,
-        category: String,
-        description: String,
-        image: String
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Cập nhật sản phẩm thành công",
-    data: {
-        _id: String,
-        name: String,
-        price: Number,
-        category: String,
-        description: String,
-        image: String
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Xóa sản phẩm thành công",
-    data: {
-        _id: String,
-        name: String,
-        price: Number,
-        category: String,
-        description: String
-        image: String
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    message: "Truy xuất danh sách sản phẩm thành công",
-    data: [
-        {
-            _id: String,
-            name: String,
-            price: Number,
-            category: String,
-            description: String
-            image: String
-        },
-        ...
-    ]
-}</t>
-  </si>
-  <si>
-    <t>Đổi mật khẩu</t>
-  </si>
-  <si>
-    <t>{
-    message: "Đổi mật khẩu thành công",
-    data: {
-        _id: String,
-        username: String,
-        password: String
+        phone: String,
+        address: String,
+        totalPrice: Number,
+        status: "waiting",
+        details: [
+            {
+                name: String,
+                unitPrice: Number,
+                quantity: Number,
+                totalPrice: Number
+            },
+            ...
+        ],
+        createdAt: Date
     }
 }</t>
   </si>
@@ -567,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -587,6 +613,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -918,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2C3AC2-1953-4FAC-AF4F-9C90EBFE5397}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -932,28 +961,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
@@ -961,7 +990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="214.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="231" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -975,13 +1004,13 @@
         <v>11</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="198" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="214.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -995,15 +1024,15 @@
         <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="214.5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="231" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -1015,10 +1044,10 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1038,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6667C6A-6953-4FC7-8876-B66BC364041C}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1052,28 +1081,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
@@ -1081,76 +1110,76 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="198" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="214.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="247.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="264" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="198" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="214.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="181.5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="198" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1169,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A00F7CC-FA3E-40A3-89A7-D8F82A1D3AF4}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1183,28 +1212,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
@@ -1212,58 +1241,58 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="181.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1282,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840C4747-A28F-4E20-93B1-6EA552B50E7E}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1296,28 +1325,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
@@ -1325,78 +1354,78 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="363" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="379.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="264" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="379.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="396" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="379.5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="396" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1415,54 +1444,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BEE959-898E-474C-85ED-6414D8A91754}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="6" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="42.85546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8" t="s">
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>9</v>
@@ -1474,18 +1504,18 @@
         <v>60</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="181.5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="198" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
@@ -1493,42 +1523,42 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1540,5 +1570,6 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add badge to cart icon + some minor fixes
</commit_message>
<xml_diff>
--- a/MilkTea.xlsx
+++ b/MilkTea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MilkTea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2453D496-5E44-46D9-9B13-5EC7E7803329}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C60F93-9D8E-4AB2-9D48-01639F4B53A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{B37F149E-6956-44B3-A4D9-19C02EF6CB64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{B37F149E-6956-44B3-A4D9-19C02EF6CB64}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>USE CASE</t>
   </si>
@@ -552,6 +552,9 @@
         createdAt: Date
     }
 }</t>
+  </si>
+  <si>
+    <t>Lấy danh sách quản trị viên</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840C4747-A28F-4E20-93B1-6EA552B50E7E}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1472,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BEE959-898E-474C-85ED-6414D8A91754}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="4" spans="1:6" ht="198" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Add search bar to navigation header, add admin login
</commit_message>
<xml_diff>
--- a/MilkTea.xlsx
+++ b/MilkTea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MilkTea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C60F93-9D8E-4AB2-9D48-01639F4B53A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17953B6-D88A-47B1-95F9-09C626F8355D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{B37F149E-6956-44B3-A4D9-19C02EF6CB64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
   <si>
     <t>USE CASE</t>
   </si>
@@ -555,6 +555,23 @@
   </si>
   <si>
     <t>Lấy danh sách quản trị viên</t>
+  </si>
+  <si>
+    <t>Đăng nhập tài khoản quản trị viên</t>
+  </si>
+  <si>
+    <t>/admins/login</t>
+  </si>
+  <si>
+    <t>{
+    error: false,
+    message: "Đăng nhập thành công",
+    data: {
+        _id: String,
+        username: String,
+        password: String
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -978,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2C3AC2-1953-4FAC-AF4F-9C90EBFE5397}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1473,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BEE959-898E-474C-85ED-6414D8A91754}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1538,57 +1555,77 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="198" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="198" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>